<commit_message>
Versão com viagens circulares
</commit_message>
<xml_diff>
--- a/data/raw/arquivo_de_exemplo.xlsx
+++ b/data/raw/arquivo_de_exemplo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SMTR\Repositórios - SMTR\algoritmo_recursos_individuais\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD7E0FA-231B-4601-885E-01A246E88E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426EA8A2-DD49-4303-9794-76B54170522D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{677A12E8-7F7C-4ABD-8CEC-F31908A8329F}"/>
+    <workbookView xWindow="-7125" yWindow="3030" windowWidth="14400" windowHeight="7800" xr2:uid="{677A12E8-7F7C-4ABD-8CEC-F31908A8329F}"/>
   </bookViews>
   <sheets>
     <sheet name="amostra" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>data</t>
   </si>
@@ -63,13 +63,16 @@
     <t>B51612</t>
   </si>
   <si>
-    <t>LECD50</t>
-  </si>
-  <si>
-    <t>A27684</t>
-  </si>
-  <si>
     <t>flag_reprocessamento</t>
+  </si>
+  <si>
+    <t>C47689</t>
+  </si>
+  <si>
+    <t>11:44:00</t>
+  </si>
+  <si>
+    <t>11:49:00</t>
   </si>
 </sst>
 </file>
@@ -77,9 +80,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,17 +104,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -157,35 +153,37 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -505,234 +503,240 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44971</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.67569444444444438</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D2" s="7">
+        <v>917</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>45084</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.32777777777777778</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.34861111111111115</v>
+      </c>
+      <c r="D3" s="7">
+        <v>712</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>45099</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.7715277777777777</v>
+      </c>
+      <c r="D4" s="7">
+        <v>805</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>45099</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.85277777777777775</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="D5" s="7">
+        <v>301</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>45102</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.81388888888888899</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="D6" s="7">
+        <v>847</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>45121</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.2902777777777778</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.33749999999999997</v>
+      </c>
+      <c r="D7" s="7">
+        <v>775</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>45113</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.4770833333333333</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.48194444444444445</v>
+      </c>
+      <c r="D8" s="7">
+        <v>844</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>45113</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.48819444444444443</v>
+      </c>
+      <c r="D9" s="7">
+        <v>844</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>45113</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="3">
-        <v>44971</v>
-      </c>
-      <c r="B2" s="9">
-        <v>0.67569444444444438</v>
-      </c>
-      <c r="C2" s="9">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="D2" s="4">
-        <v>917</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="3">
-        <v>45084</v>
-      </c>
-      <c r="B3" s="9">
-        <v>0.32777777777777778</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0.34861111111111115</v>
-      </c>
-      <c r="D3" s="4">
-        <v>712</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="3">
-        <v>45099</v>
-      </c>
-      <c r="B4" s="9">
-        <v>0.74375000000000002</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0.7715277777777777</v>
-      </c>
-      <c r="D4" s="4">
-        <v>805</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="3">
-        <v>45099</v>
-      </c>
-      <c r="B5" s="9">
-        <v>0.85277777777777775</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0.88541666666666663</v>
-      </c>
-      <c r="D5" s="4">
-        <v>301</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="3">
-        <v>45102</v>
-      </c>
-      <c r="B6" s="9">
-        <v>0.81388888888888899</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0.82500000000000007</v>
-      </c>
-      <c r="D6" s="4">
-        <v>847</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="3">
-        <v>45121</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0.2902777777777778</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0.33749999999999997</v>
-      </c>
-      <c r="D7" s="4">
-        <v>775</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="6">
-        <v>44971</v>
-      </c>
-      <c r="B8" s="10">
-        <v>0.16319444444444445</v>
-      </c>
-      <c r="C8" s="10">
-        <v>0.16805555555555554</v>
-      </c>
-      <c r="D8" s="4">
-        <v>848</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="6">
-        <v>45121</v>
-      </c>
-      <c r="B9" s="10">
-        <v>0.84722222222222221</v>
-      </c>
-      <c r="C9" s="10">
-        <v>0.85555555555555562</v>
-      </c>
-      <c r="D9" s="4">
-        <v>350</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="6">
-        <v>44817</v>
-      </c>
-      <c r="B10" s="11">
-        <v>0.53611111111111109</v>
-      </c>
-      <c r="C10" s="11">
-        <v>0.56527777777777777</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>12</v>
+      <c r="C10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="7">
+        <v>844</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="G11" s="1"/>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Otimização do algoritmo e mudança de ordem
</commit_message>
<xml_diff>
--- a/data/raw/arquivo_de_exemplo.xlsx
+++ b/data/raw/arquivo_de_exemplo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SMTR\Repositórios - SMTR\algoritmo_recursos_individuais\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D089DB9-4DD8-4CC3-BE17-427F62A83123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE50DF7-1F38-46B3-B656-9DB531DC1865}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{677A12E8-7F7C-4ABD-8CEC-F31908A8329F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>data</t>
   </si>
@@ -42,33 +42,12 @@
     <t>id_veiculo</t>
   </si>
   <si>
-    <t>C44530</t>
-  </si>
-  <si>
-    <t>C50068</t>
-  </si>
-  <si>
-    <t>A50002</t>
-  </si>
-  <si>
-    <t>D53557</t>
-  </si>
-  <si>
-    <t>B27036</t>
-  </si>
-  <si>
     <t>sentido</t>
   </si>
   <si>
-    <t>B51612</t>
-  </si>
-  <si>
     <t>flag_reprocessamento</t>
   </si>
   <si>
-    <t>C47689</t>
-  </si>
-  <si>
     <t>11:44:00</t>
   </si>
   <si>
@@ -76,9 +55,6 @@
   </si>
   <si>
     <t>LECD50</t>
-  </si>
-  <si>
-    <t>A27684</t>
   </si>
 </sst>
 </file>
@@ -503,7 +479,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,13 +507,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -554,8 +530,8 @@
         <v>917</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
+      <c r="F2" s="4">
+        <v>51612</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -575,8 +551,8 @@
         <v>712</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>5</v>
+      <c r="F3" s="4">
+        <v>44530</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -596,8 +572,8 @@
         <v>805</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
+      <c r="F4" s="4">
+        <v>50068</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -617,8 +593,8 @@
         <v>301</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>7</v>
+      <c r="F5" s="4">
+        <v>50002</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -638,8 +614,8 @@
         <v>847</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>8</v>
+      <c r="F6" s="4">
+        <v>53557</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -659,8 +635,8 @@
         <v>775</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>9</v>
+      <c r="F7" s="4">
+        <v>27036</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -680,8 +656,8 @@
         <v>844</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="7" t="s">
-        <v>13</v>
+      <c r="F8" s="7">
+        <v>47689</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -701,8 +677,8 @@
         <v>844</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="7" t="s">
-        <v>13</v>
+      <c r="F9" s="7">
+        <v>47689</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -713,17 +689,17 @@
         <v>45113</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D10" s="4">
         <v>844</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="7" t="s">
-        <v>13</v>
+      <c r="F10" s="7">
+        <v>47689</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -740,11 +716,11 @@
         <v>0.27083333333333331</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="7" t="s">
-        <v>17</v>
+      <c r="F11" s="7">
+        <v>27684</v>
       </c>
       <c r="G11" s="4">
         <v>1</v>

</xml_diff>